<commit_message>
update uc2_plan , add Login workflow
</commit_message>
<xml_diff>
--- a/docs/uc2_plan.xlsx
+++ b/docs/uc2_plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>S.No</t>
   </si>
@@ -103,13 +103,31 @@
     <t xml:space="preserve"> create new views in native iOS app with UI design</t>
   </si>
   <si>
-    <t>zhangxiaodong</t>
-  </si>
-  <si>
-    <t>both</t>
-  </si>
-  <si>
     <t>IDC</t>
+  </si>
+  <si>
+    <t>liubin&amp;zhangxiaodong</t>
+  </si>
+  <si>
+    <t>Investigat the Jawbone &amp; Nick API, select wearable device</t>
+  </si>
+  <si>
+    <t>to the end</t>
+  </si>
+  <si>
+    <t>IDC want to use Nick+, but SDK can't get</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Make lib for QRScan and iBeacons</t>
+  </si>
+  <si>
+    <t>Create Jawbone Login View base on app of Q1 and Jawbone developer account</t>
+  </si>
+  <si>
+    <t>Send the Screenshot to IDC which is Jawbone Login View.</t>
   </si>
 </sst>
 </file>
@@ -654,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -757,151 +775,181 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" s="4">
-        <v>18</v>
-      </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+        <v>24</v>
+      </c>
+      <c r="E4" s="23">
+        <v>41984</v>
+      </c>
+      <c r="F4" s="23">
+        <v>41989</v>
+      </c>
       <c r="G4" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>20</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="H4" s="11"/>
       <c r="I4" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4">
-        <v>9</v>
-      </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+        <v>32</v>
+      </c>
+      <c r="E5" s="23">
+        <v>41990</v>
+      </c>
+      <c r="F5" s="23">
+        <v>41996</v>
+      </c>
       <c r="G5" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="I5" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4">
-        <v>36</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+        <v>48</v>
+      </c>
+      <c r="E6" s="23">
+        <v>41997</v>
+      </c>
+      <c r="F6" s="23">
+        <v>42004</v>
+      </c>
       <c r="G6" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="4">
-        <v>9</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+        <v>18</v>
+      </c>
+      <c r="E7" s="23">
+        <v>42009</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="G7" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>27</v>
-      </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+        <v>9</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="24" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H8" s="11"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" s="4">
-        <v>18</v>
-      </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+        <v>36</v>
+      </c>
+      <c r="E9" s="23">
+        <v>42009</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="G9" s="24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4">
-        <v>3</v>
-      </c>
-      <c r="D10" s="4">
-        <v>27</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
       <c r="G10" s="24" t="s">
@@ -910,80 +958,94 @@
       <c r="H10" s="11"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="4">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4">
-        <v>36</v>
-      </c>
+      <c r="B11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="H11" s="11"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="9"/>
+    <row r="12" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="5"/>
+      <c r="G12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="11"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="9"/>
+    <row r="13" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="11"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
+    <row r="14" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="10"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="8"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
       <c r="G16" s="24"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1005,7 +1067,7 @@
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
       <c r="G18" s="24"/>
-      <c r="H18" s="11"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1016,7 +1078,7 @@
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
       <c r="G19" s="24"/>
-      <c r="H19" s="11"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1030,25 +1092,58 @@
       <c r="H20" s="8"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="16"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="17">
-        <f>SUM(C2:C21)</f>
-        <v>24.5</v>
-      </c>
-      <c r="D22" s="17">
-        <f>SUM(D2:D21)</f>
-        <v>220</v>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="17">
+        <f>SUM(C2:C24)</f>
+        <v>25.5</v>
+      </c>
+      <c r="D25" s="17">
+        <f>SUM(D2:D24)</f>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>